<commit_message>
ADC Schematics Completed and Folder Modifications
</commit_message>
<xml_diff>
--- a/Drawings/Target3001/Header_Tables.xlsx
+++ b/Drawings/Target3001/Header_Tables.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develop\FYP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develop\FYP\Drawings\Target3001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6659B9-D727-40CE-BCFE-A4DF2FE27AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912D3CEA-6F9D-413A-B4F4-8191958CE36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="31800" xr2:uid="{1169C5DA-BBE0-4116-BBF3-A5E12840D734}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="28800" windowHeight="31800" activeTab="3" xr2:uid="{1169C5DA-BBE0-4116-BBF3-A5E12840D734}"/>
   </bookViews>
   <sheets>
     <sheet name="DAC_And_CS_Header" sheetId="1" r:id="rId1"/>
     <sheet name="DAC_OUTPUT" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="ADC_Analog_Output" sheetId="3" r:id="rId3"/>
+    <sheet name="ADC_Header" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="110">
   <si>
     <t>Header Pin</t>
   </si>
@@ -284,13 +285,97 @@
   </si>
   <si>
     <t xml:space="preserve">    D1_MCP4811_VOUTB</t>
+  </si>
+  <si>
+    <t>MCP3008 Connection</t>
+  </si>
+  <si>
+    <t>U1_ADC_CH7</t>
+  </si>
+  <si>
+    <t>U2_ADC_CH0</t>
+  </si>
+  <si>
+    <t>U1_ADC_CH6</t>
+  </si>
+  <si>
+    <t>U1_ADC_CH1</t>
+  </si>
+  <si>
+    <t>U1_ADC_CH5</t>
+  </si>
+  <si>
+    <t>U1_ADC_CH2</t>
+  </si>
+  <si>
+    <t>U2_ADC_CH2</t>
+  </si>
+  <si>
+    <t>U2_ADC_CH3</t>
+  </si>
+  <si>
+    <t>U2_ADC_CH4</t>
+  </si>
+  <si>
+    <t>U2_ADC_CH5</t>
+  </si>
+  <si>
+    <t>U2_ADC_CH6</t>
+  </si>
+  <si>
+    <t>U2_ADC_CH7</t>
+  </si>
+  <si>
+    <t>U1_ADC_CH3</t>
+  </si>
+  <si>
+    <t>U1_ADC_CH4</t>
+  </si>
+  <si>
+    <t>U1_ADC_CH0</t>
+  </si>
+  <si>
+    <t>MCP3008 U1</t>
+  </si>
+  <si>
+    <t>MCP3008 U2</t>
+  </si>
+  <si>
+    <t>SPI_Data_In (Duo)</t>
+  </si>
+  <si>
+    <t>Din</t>
+  </si>
+  <si>
+    <t>CLK</t>
+  </si>
+  <si>
+    <t>Vref</t>
+  </si>
+  <si>
+    <t>CS_U2</t>
+  </si>
+  <si>
+    <t>CS_U1</t>
+  </si>
+  <si>
+    <t>Dout_U2</t>
+  </si>
+  <si>
+    <t>Dout_U1</t>
+  </si>
+  <si>
+    <t>A&amp;D_GND</t>
+  </si>
+  <si>
+    <t>ADC_Header_1*12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +394,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -883,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFC85674-D21E-4BE3-BC4A-758C244E3C46}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,7 +1224,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+      <selection activeCell="C21" sqref="A1:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,12 +1473,511 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41BC11EE-7895-4E9E-A2BE-F36EFA9FFEFC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="17" t="str">
+        <f xml:space="preserve"> "MCP3008_" &amp; B2</f>
+        <v>MCP3008_U1_ADC_CH7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="17" t="str">
+        <f t="shared" ref="C3:C17" si="0" xml:space="preserve"> "MCP3008_" &amp; B3</f>
+        <v>MCP3008_U2_ADC_CH0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>MCP3008_U1_ADC_CH6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>MCP3008_U1_ADC_CH1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>MCP3008_U1_ADC_CH5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>MCP3008_U2_ADC_CH2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>MCP3008_U1_ADC_CH4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>MCP3008_U2_ADC_CH3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>MCP3008_U1_ADC_CH3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>MCP3008_U2_ADC_CH4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>MCP3008_U1_ADC_CH2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>MCP3008_U2_ADC_CH5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>MCP3008_U1_ADC_CH1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>MCP3008_U2_ADC_CH6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>MCP3008_U1_ADC_CH0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>MCP3008_U2_ADC_CH7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E314D53A-82FA-428C-ABAB-4BBAF6D8ADCE}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>